<commit_message>
[Ankita]Add:Login Facebook using TestNg Parameter
</commit_message>
<xml_diff>
--- a/src/main/resources/Signin.xlsx
+++ b/src/main/resources/Signin.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>ankitakhairnar10@gmail.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -27,7 +24,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>ankoo1711997</t>
+    <t>latikakhairnar10@gmail.com</t>
+  </si>
+  <si>
+    <t>latika@123</t>
   </si>
 </sst>
 </file>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,23 +391,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>